<commit_message>
add iq y urgengencia v0.1.1
</commit_message>
<xml_diff>
--- a/fhir/ig/iq/StructureDefinition-AllergyIntoleranceIniciarLE.xlsx
+++ b/fhir/ig/iq/StructureDefinition-AllergyIntoleranceIniciarLE.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>0.1.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-16T14:50:11-03:00</t>
+    <t>2024-12-17T10:27:17-03:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>